<commit_message>
Projeto final do curso Python do IPEA v2 (atualizado com plot e gera arquivo BD3.xlsx)
</commit_message>
<xml_diff>
--- a/BD3.xlsx
+++ b/BD3.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.286753035834244</v>
+        <v>4.35119740180176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projeto final do curso Python do IPEA v3 (com dicionario)
</commit_message>
<xml_diff>
--- a/BD3.xlsx
+++ b/BD3.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.05</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.302215855677225</v>
+        <v>4.568483200132085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projeto final do curso Python do IPEA v3 (atualizado)
</commit_message>
<xml_diff>
--- a/BD3.xlsx
+++ b/BD3.xlsx
@@ -385,7 +385,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>4.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -393,7 +393,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>4.29845246718807</v>
+        <v>3.570679587824878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>